<commit_message>
Fixed quiz 2 link
</commit_message>
<xml_diff>
--- a/calendar/Calendar.xlsx
+++ b/calendar/Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabehope/Documents/DataViz/calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21584ABC-3950-4343-908B-F53BEB119E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEEB93A-4E61-EE4B-972D-805BCB8F2BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="1540" windowWidth="29400" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="760" windowWidth="29400" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,9 +504,6 @@
     <t>Inference</t>
   </si>
   <si>
-    <t>[Notebook](https://drive.google.com/file/d/1o9U6DYQAs9DRt1ZX9YmHCZzXEtGrlbIm/view?usp=sharing)  Gradescope TBA</t>
-  </si>
-  <si>
     <t>Multi-variable data</t>
   </si>
   <si>
@@ -538,6 +535,9 @@
   </si>
   <si>
     <t>Read before lecture</t>
+  </si>
+  <si>
+    <t>[Notebook](https://drive.google.com/file/d/1PcoV5ksM3Ezu6amxVHnS5Al4-GGCuvWI/view?usp=sharing)  Gradescope TBA</t>
   </si>
 </sst>
 </file>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="48" customHeight="1"/>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>61</v>
@@ -2212,14 +2212,14 @@
         <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="48" customHeight="1">
@@ -2237,10 +2237,10 @@
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="48" customHeight="1">
@@ -2292,14 +2292,14 @@
         <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="48" customHeight="1">
@@ -2313,14 +2313,14 @@
         <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="48" customHeight="1">

</xml_diff>

<commit_message>
Updated quizzes 2 & 3
</commit_message>
<xml_diff>
--- a/calendar/Calendar.xlsx
+++ b/calendar/Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabehope/Documents/DataViz/calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEEB93A-4E61-EE4B-972D-805BCB8F2BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8CB0B9-8D4B-E644-941B-E029EF51B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="760" windowWidth="29400" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1620" windowWidth="29400" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,9 +507,6 @@
     <t>Multi-variable data</t>
   </si>
   <si>
-    <t>[Notebook](https://drive.google.com/file/d/1EblgjomptOWZYVQYQNe8KXLkhxFpnDtt/view?usp=sharing) Gradescope TBA</t>
-  </si>
-  <si>
     <t>Multi-variable visualization</t>
   </si>
   <si>
@@ -537,7 +534,10 @@
     <t>Read before lecture</t>
   </si>
   <si>
-    <t>[Notebook](https://drive.google.com/file/d/1PcoV5ksM3Ezu6amxVHnS5Al4-GGCuvWI/view?usp=sharing)  Gradescope TBA</t>
+    <t>[Notebook](https://drive.google.com/file/d/1EblgjomptOWZYVQYQNe8KXLkhxFpnDtt/view?usp=sharing) [Data](../modules/02-Multiple-variables/assignments/data/data.zip) Gradescope TBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Notebook](https://drive.google.com/file/d/1PcoV5ksM3Ezu6amxVHnS5Al4-GGCuvWI/view?usp=sharing)  [Gradescope](https://www.gradescope.com/courses/842824/assignments/5189929) </t>
   </si>
 </sst>
 </file>
@@ -1768,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>61</v>
@@ -2212,14 +2212,14 @@
         <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="48" customHeight="1">
@@ -2240,7 +2240,7 @@
         <v>121</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="48" customHeight="1">
@@ -2296,10 +2296,10 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="48" customHeight="1">
@@ -2313,14 +2313,14 @@
         <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="48" customHeight="1">

</xml_diff>